<commit_message>
Changes for Ledger files
Changes for Ledger files
</commit_message>
<xml_diff>
--- a/01_Requirements/LedgerTypes/01_Bank Ledger creation.xlsx
+++ b/01_Requirements/LedgerTypes/01_Bank Ledger creation.xlsx
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
   <si>
     <t xml:space="preserve">This screen is same for all Individuals/Firms/ HUF's/ LLP/ Company </t>
   </si>
@@ -69,41 +69,32 @@
     <t>Current / Savings/ CC/ ODC/FD/RD/ Loan</t>
   </si>
   <si>
-    <t>Drop down box of above nature of A/c's</t>
-  </si>
-  <si>
     <t xml:space="preserve">If CC/ FD/ RD / Loan is Selected :- </t>
   </si>
   <si>
     <t>Interest Rate</t>
   </si>
   <si>
-    <t xml:space="preserve">Cheque Book Details </t>
-  </si>
-  <si>
-    <t xml:space="preserve">( Cheque Book Numbering) </t>
-  </si>
-  <si>
-    <t xml:space="preserve">First Cheque No </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Cheque No </t>
-  </si>
-  <si>
-    <t>No. of Cheque Leafs</t>
-  </si>
-  <si>
-    <t>(0+ above Cheque No)</t>
-  </si>
-  <si>
     <t xml:space="preserve">Opening Balance </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Address </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Location </t>
+  </si>
+  <si>
+    <t>Pin code</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Contact No </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="3">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -246,7 +237,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -263,18 +254,18 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -282,21 +273,6 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -622,13 +598,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="E2:K29"/>
+  <dimension ref="E2:K23"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A8" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E29" sqref="E29"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="24.95" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="24.95" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="4" width="9.140625" style="1"/>
     <col min="5" max="5" width="73" style="1" customWidth="1"/>
@@ -636,28 +612,28 @@
     <col min="7" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="5:11" ht="24.95" customHeight="1">
+    <row r="2" spans="5:11" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="E2" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="5:11" ht="24.95" customHeight="1" thickBot="1"/>
-    <row r="4" spans="5:11" ht="24.95" customHeight="1" thickBot="1">
-      <c r="E4" s="18" t="s">
+    <row r="3" spans="5:11" ht="24.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="4" spans="5:11" ht="24.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E4" s="13" t="s">
         <v>1</v>
       </c>
-      <c r="F4" s="19"/>
-      <c r="G4" s="19"/>
-      <c r="H4" s="19"/>
-      <c r="I4" s="19"/>
-      <c r="J4" s="19"/>
-      <c r="K4" s="20"/>
-    </row>
-    <row r="5" spans="5:11" ht="24.95" customHeight="1" thickBot="1">
+      <c r="F4" s="14"/>
+      <c r="G4" s="14"/>
+      <c r="H4" s="14"/>
+      <c r="I4" s="14"/>
+      <c r="J4" s="14"/>
+      <c r="K4" s="15"/>
+    </row>
+    <row r="5" spans="5:11" ht="24.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="E5" s="2"/>
       <c r="K5" s="3"/>
     </row>
-    <row r="6" spans="5:11" ht="24.95" customHeight="1" thickBot="1">
+    <row r="6" spans="5:11" ht="24.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="E6" s="4" t="s">
         <v>2</v>
       </c>
@@ -669,15 +645,15 @@
       <c r="J6" s="11"/>
       <c r="K6" s="12"/>
     </row>
-    <row r="7" spans="5:11" ht="24.95" customHeight="1" thickBot="1">
+    <row r="7" spans="5:11" ht="24.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="E7" s="5"/>
-      <c r="G7" s="6"/>
-      <c r="H7" s="6"/>
-      <c r="I7" s="6"/>
-      <c r="J7" s="6"/>
-      <c r="K7" s="7"/>
-    </row>
-    <row r="8" spans="5:11" ht="24.95" customHeight="1" thickBot="1">
+      <c r="G7" s="8"/>
+      <c r="H7" s="8"/>
+      <c r="I7" s="8"/>
+      <c r="J7" s="8"/>
+      <c r="K7" s="9"/>
+    </row>
+    <row r="8" spans="5:11" ht="24.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="E8" s="5" t="s">
         <v>4</v>
       </c>
@@ -687,200 +663,161 @@
       <c r="J8" s="11"/>
       <c r="K8" s="12"/>
     </row>
-    <row r="9" spans="5:11" ht="24.95" customHeight="1" thickBot="1">
+    <row r="9" spans="5:11" ht="24.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="E9" s="5"/>
-      <c r="G9" s="6"/>
-      <c r="H9" s="6"/>
-      <c r="I9" s="6"/>
-      <c r="J9" s="6"/>
-      <c r="K9" s="7"/>
-    </row>
-    <row r="10" spans="5:11" ht="24.95" customHeight="1" thickBot="1">
+      <c r="G9" s="8"/>
+      <c r="H9" s="8"/>
+      <c r="I9" s="8"/>
+      <c r="J9" s="8"/>
+      <c r="K9" s="9"/>
+    </row>
+    <row r="10" spans="5:11" ht="24.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="E10" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="G10" s="10"/>
+      <c r="G10" s="10" t="s">
+        <v>13</v>
+      </c>
       <c r="H10" s="11"/>
       <c r="I10" s="11"/>
       <c r="J10" s="11"/>
       <c r="K10" s="12"/>
     </row>
-    <row r="11" spans="5:11" ht="24.95" customHeight="1" thickBot="1">
+    <row r="11" spans="5:11" ht="24.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="E11" s="5"/>
-      <c r="G11" s="6"/>
-      <c r="H11" s="6"/>
-      <c r="I11" s="6"/>
-      <c r="J11" s="6"/>
-      <c r="K11" s="7"/>
-    </row>
-    <row r="12" spans="5:11" ht="24.95" customHeight="1" thickBot="1">
-      <c r="E12" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="G12" s="10"/>
+      <c r="G11" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="H11" s="11"/>
+      <c r="I11" s="11"/>
+      <c r="J11" s="11"/>
+      <c r="K11" s="12"/>
+    </row>
+    <row r="12" spans="5:11" ht="24.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E12" s="5"/>
+      <c r="G12" s="10" t="s">
+        <v>15</v>
+      </c>
       <c r="H12" s="11"/>
       <c r="I12" s="11"/>
       <c r="J12" s="11"/>
       <c r="K12" s="12"/>
     </row>
-    <row r="13" spans="5:11" ht="24.95" customHeight="1" thickBot="1">
+    <row r="13" spans="5:11" ht="24.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="E13" s="5"/>
-      <c r="G13" s="6"/>
-      <c r="H13" s="6"/>
-      <c r="I13" s="6"/>
-      <c r="J13" s="6"/>
-      <c r="K13" s="7"/>
-    </row>
-    <row r="14" spans="5:11" ht="24.95" customHeight="1" thickBot="1">
-      <c r="E14" s="5" t="s">
+      <c r="G13" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="H13" s="11"/>
+      <c r="I13" s="11"/>
+      <c r="J13" s="11"/>
+      <c r="K13" s="12"/>
+    </row>
+    <row r="14" spans="5:11" ht="24.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E14" s="5"/>
+      <c r="G14" s="8"/>
+      <c r="H14" s="8"/>
+      <c r="I14" s="8"/>
+      <c r="J14" s="8"/>
+      <c r="K14" s="9"/>
+    </row>
+    <row r="15" spans="5:11" ht="24.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E15" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="G15" s="10"/>
+      <c r="H15" s="11"/>
+      <c r="I15" s="11"/>
+      <c r="J15" s="11"/>
+      <c r="K15" s="12"/>
+    </row>
+    <row r="16" spans="5:11" ht="24.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E16" s="5"/>
+      <c r="G16" s="8"/>
+      <c r="H16" s="8"/>
+      <c r="I16" s="8"/>
+      <c r="J16" s="8"/>
+      <c r="K16" s="9"/>
+    </row>
+    <row r="17" spans="5:11" ht="24.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E17" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="G14" s="10"/>
-      <c r="H14" s="11"/>
-      <c r="I14" s="11"/>
-      <c r="J14" s="11"/>
-      <c r="K14" s="12"/>
-    </row>
-    <row r="15" spans="5:11" ht="24.95" customHeight="1" thickBot="1">
-      <c r="E15" s="5"/>
-      <c r="G15" s="6"/>
-      <c r="H15" s="6"/>
-      <c r="I15" s="6"/>
-      <c r="J15" s="6"/>
-      <c r="K15" s="7"/>
-    </row>
-    <row r="16" spans="5:11" ht="24.95" customHeight="1" thickBot="1">
-      <c r="E16" s="5" t="s">
+      <c r="G17" s="10"/>
+      <c r="H17" s="11"/>
+      <c r="I17" s="11"/>
+      <c r="J17" s="11"/>
+      <c r="K17" s="12"/>
+    </row>
+    <row r="18" spans="5:11" ht="24.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E18" s="5"/>
+      <c r="G18" s="8"/>
+      <c r="H18" s="8"/>
+      <c r="I18" s="8"/>
+      <c r="J18" s="8"/>
+      <c r="K18" s="9"/>
+    </row>
+    <row r="19" spans="5:11" ht="24.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E19" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="G16" s="10" t="s">
+      <c r="G19" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="H16" s="11"/>
-      <c r="I16" s="11"/>
-      <c r="J16" s="11"/>
-      <c r="K16" s="12"/>
-    </row>
-    <row r="17" spans="5:11" ht="24.95" customHeight="1">
-      <c r="E17" s="5"/>
-      <c r="G17" s="6"/>
-      <c r="H17" s="6"/>
-      <c r="I17" s="6"/>
-      <c r="J17" s="6"/>
-      <c r="K17" s="7"/>
-    </row>
-    <row r="18" spans="5:11" ht="24.95" customHeight="1">
-      <c r="E18" s="5"/>
-      <c r="G18" s="13" t="s">
+      <c r="H19" s="11"/>
+      <c r="I19" s="11"/>
+      <c r="J19" s="11"/>
+      <c r="K19" s="12"/>
+    </row>
+    <row r="20" spans="5:11" ht="24.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E20" s="5"/>
+      <c r="G20" s="8"/>
+      <c r="H20" s="8"/>
+      <c r="I20" s="8"/>
+      <c r="J20" s="8"/>
+      <c r="K20" s="9"/>
+    </row>
+    <row r="21" spans="5:11" ht="24.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E21" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="H18" s="13"/>
-      <c r="I18" s="13"/>
-      <c r="J18" s="13"/>
-      <c r="K18" s="14"/>
-    </row>
-    <row r="19" spans="5:11" ht="24.95" customHeight="1" thickBot="1">
-      <c r="E19" s="5"/>
-      <c r="G19" s="6"/>
-      <c r="H19" s="6"/>
-      <c r="I19" s="6"/>
-      <c r="J19" s="6"/>
-      <c r="K19" s="7"/>
-    </row>
-    <row r="20" spans="5:11" ht="24.95" customHeight="1" thickBot="1">
-      <c r="E20" s="5" t="s">
+      <c r="G21" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="G20" s="10" t="s">
+      <c r="H21" s="11"/>
+      <c r="I21" s="11"/>
+      <c r="J21" s="11"/>
+      <c r="K21" s="12"/>
+    </row>
+    <row r="22" spans="5:11" ht="24.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E22" s="5"/>
+      <c r="K22" s="3"/>
+    </row>
+    <row r="23" spans="5:11" ht="24.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E23" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="H20" s="11"/>
-      <c r="I20" s="11"/>
-      <c r="J20" s="11"/>
-      <c r="K20" s="12"/>
-    </row>
-    <row r="21" spans="5:11" ht="24.95" customHeight="1" thickBot="1">
-      <c r="E21" s="5"/>
-      <c r="K21" s="3"/>
-    </row>
-    <row r="22" spans="5:11" ht="24.95" customHeight="1" thickBot="1">
-      <c r="E22" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="G22" s="10" t="s">
-        <v>14</v>
-      </c>
-      <c r="H22" s="11"/>
-      <c r="I22" s="11"/>
-      <c r="J22" s="11"/>
-      <c r="K22" s="12"/>
-    </row>
-    <row r="23" spans="5:11" ht="24.95" customHeight="1" thickBot="1">
-      <c r="E23" s="5"/>
-      <c r="K23" s="3"/>
-    </row>
-    <row r="24" spans="5:11" ht="24.95" customHeight="1" thickBot="1">
-      <c r="E24" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="G24" s="10" t="s">
-        <v>16</v>
-      </c>
-      <c r="H24" s="11"/>
-      <c r="I24" s="11"/>
-      <c r="J24" s="11"/>
-      <c r="K24" s="12"/>
-    </row>
-    <row r="25" spans="5:11" ht="24.95" customHeight="1" thickBot="1">
-      <c r="E25" s="5"/>
-      <c r="K25" s="3"/>
-    </row>
-    <row r="26" spans="5:11" ht="24.95" customHeight="1" thickBot="1">
-      <c r="E26" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="G26" s="15" t="s">
-        <v>18</v>
-      </c>
-      <c r="H26" s="16"/>
-      <c r="I26" s="16"/>
-      <c r="J26" s="16"/>
-      <c r="K26" s="17"/>
-    </row>
-    <row r="27" spans="5:11" ht="24.95" customHeight="1">
-      <c r="E27" s="5"/>
-      <c r="K27" s="3"/>
-    </row>
-    <row r="28" spans="5:11" ht="24.95" customHeight="1" thickBot="1">
-      <c r="E28" s="5"/>
-      <c r="K28" s="3"/>
-    </row>
-    <row r="29" spans="5:11" ht="24.95" customHeight="1" thickBot="1">
-      <c r="E29" s="8" t="s">
-        <v>19</v>
-      </c>
-      <c r="F29" s="9"/>
-      <c r="G29" s="10"/>
-      <c r="H29" s="11"/>
-      <c r="I29" s="11"/>
-      <c r="J29" s="11"/>
-      <c r="K29" s="12"/>
+      <c r="F23" s="7"/>
+      <c r="G23" s="10"/>
+      <c r="H23" s="11"/>
+      <c r="I23" s="11"/>
+      <c r="J23" s="11"/>
+      <c r="K23" s="12"/>
     </row>
   </sheetData>
-  <mergeCells count="13">
-    <mergeCell ref="G14:K14"/>
+  <mergeCells count="12">
+    <mergeCell ref="G15:K15"/>
+    <mergeCell ref="G17:K17"/>
+    <mergeCell ref="G19:K19"/>
+    <mergeCell ref="G21:K21"/>
+    <mergeCell ref="G23:K23"/>
     <mergeCell ref="E4:K4"/>
     <mergeCell ref="G6:K6"/>
     <mergeCell ref="G8:K8"/>
     <mergeCell ref="G10:K10"/>
     <mergeCell ref="G12:K12"/>
-    <mergeCell ref="G29:K29"/>
-    <mergeCell ref="G16:K16"/>
-    <mergeCell ref="G18:K18"/>
-    <mergeCell ref="G20:K20"/>
-    <mergeCell ref="G22:K22"/>
-    <mergeCell ref="G24:K24"/>
-    <mergeCell ref="G26:K26"/>
+    <mergeCell ref="G11:K11"/>
+    <mergeCell ref="G13:K13"/>
   </mergeCells>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0.11811023622047245" right="0.31496062992125984" top="0.15748031496062992" bottom="0.15748031496062992" header="0.31496062992125984" footer="0.31496062992125984"/>

</xml_diff>